<commit_message>
primeros resultados 10000 vertices
</commit_message>
<xml_diff>
--- a/Resultados_final.xlsx
+++ b/Resultados_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2a76e7a69041390e/Documentos/Maestria/Primer Semestre/Análisis de Algoritmos/Taller 7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="13_ncr:1_{DBDDEC85-B02F-4011-B6FC-B2B2BD2CDE81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8441FF45-7AB9-4C17-A84B-1DB52D8CB30F}"/>
+  <xr:revisionPtr revIDLastSave="110" documentId="13_ncr:1_{DBDDEC85-B02F-4011-B6FC-B2B2BD2CDE81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50D5FCB7-A11B-4EF5-AA49-09638CF1A5D1}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="34">
   <si>
     <t>Media</t>
   </si>
@@ -123,6 +123,18 @@
   </si>
   <si>
     <t>0.083</t>
+  </si>
+  <si>
+    <t>0.1433</t>
+  </si>
+  <si>
+    <t>1410.35</t>
+  </si>
+  <si>
+    <t>0.2441</t>
+  </si>
+  <si>
+    <t>0.086</t>
   </si>
 </sst>
 </file>
@@ -316,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -336,51 +348,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -389,18 +356,62 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,6 +427,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -703,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AX30"/>
+  <dimension ref="A1:AX31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -716,8 +731,8 @@
     <col min="4" max="4" width="20.453125" customWidth="1"/>
     <col min="5" max="5" width="18.90625" customWidth="1"/>
     <col min="6" max="6" width="16.81640625" customWidth="1"/>
-    <col min="7" max="7" width="14.54296875" customWidth="1"/>
-    <col min="8" max="8" width="13.1796875" customWidth="1"/>
+    <col min="7" max="7" width="15.7265625" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.26953125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -774,147 +789,147 @@
       <c r="AX1" s="5"/>
     </row>
     <row r="2" spans="1:50" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10" t="s">
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10" t="s">
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
-      <c r="AA2" s="10" t="s">
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="AB2" s="10"/>
-      <c r="AC2" s="10"/>
-      <c r="AD2" s="10"/>
-      <c r="AE2" s="10"/>
-      <c r="AF2" s="10"/>
-      <c r="AG2" s="10"/>
-      <c r="AH2" s="10"/>
-      <c r="AI2" s="10" t="s">
+      <c r="AB2" s="18"/>
+      <c r="AC2" s="18"/>
+      <c r="AD2" s="18"/>
+      <c r="AE2" s="18"/>
+      <c r="AF2" s="18"/>
+      <c r="AG2" s="18"/>
+      <c r="AH2" s="18"/>
+      <c r="AI2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="AJ2" s="10"/>
-      <c r="AK2" s="10"/>
-      <c r="AL2" s="10"/>
-      <c r="AM2" s="10"/>
-      <c r="AN2" s="10"/>
-      <c r="AO2" s="10"/>
-      <c r="AP2" s="10"/>
-      <c r="AQ2" s="11" t="s">
+      <c r="AJ2" s="18"/>
+      <c r="AK2" s="18"/>
+      <c r="AL2" s="18"/>
+      <c r="AM2" s="18"/>
+      <c r="AN2" s="18"/>
+      <c r="AO2" s="18"/>
+      <c r="AP2" s="18"/>
+      <c r="AQ2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="AR2" s="11"/>
-      <c r="AS2" s="11"/>
-      <c r="AT2" s="11"/>
-      <c r="AU2" s="11"/>
-      <c r="AV2" s="11"/>
-      <c r="AW2" s="11"/>
-      <c r="AX2" s="11"/>
+      <c r="AR2" s="14"/>
+      <c r="AS2" s="14"/>
+      <c r="AT2" s="14"/>
+      <c r="AU2" s="14"/>
+      <c r="AV2" s="14"/>
+      <c r="AW2" s="14"/>
+      <c r="AX2" s="14"/>
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="B3" s="13"/>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11" t="s">
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11" t="s">
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11" t="s">
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11" t="s">
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
-      <c r="W3" s="11" t="s">
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="11"/>
-      <c r="Z3" s="11"/>
-      <c r="AA3" s="11" t="s">
+      <c r="X3" s="14"/>
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="14"/>
+      <c r="AA3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="AB3" s="11"/>
-      <c r="AC3" s="11"/>
-      <c r="AD3" s="11"/>
-      <c r="AE3" s="11" t="s">
+      <c r="AB3" s="14"/>
+      <c r="AC3" s="14"/>
+      <c r="AD3" s="14"/>
+      <c r="AE3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="AF3" s="11"/>
-      <c r="AG3" s="11"/>
-      <c r="AH3" s="11"/>
-      <c r="AI3" s="11" t="s">
+      <c r="AF3" s="14"/>
+      <c r="AG3" s="14"/>
+      <c r="AH3" s="14"/>
+      <c r="AI3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="AJ3" s="11"/>
-      <c r="AK3" s="11"/>
-      <c r="AL3" s="11"/>
-      <c r="AM3" s="11" t="s">
+      <c r="AJ3" s="14"/>
+      <c r="AK3" s="14"/>
+      <c r="AL3" s="14"/>
+      <c r="AM3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="AN3" s="11"/>
-      <c r="AO3" s="11"/>
-      <c r="AP3" s="11"/>
-      <c r="AQ3" s="11" t="s">
+      <c r="AN3" s="14"/>
+      <c r="AO3" s="14"/>
+      <c r="AP3" s="14"/>
+      <c r="AQ3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="AR3" s="11"/>
-      <c r="AS3" s="11"/>
-      <c r="AT3" s="11"/>
-      <c r="AU3" s="11" t="s">
+      <c r="AR3" s="14"/>
+      <c r="AS3" s="14"/>
+      <c r="AT3" s="14"/>
+      <c r="AU3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="AV3" s="11"/>
-      <c r="AW3" s="11"/>
-      <c r="AX3" s="11"/>
+      <c r="AV3" s="14"/>
+      <c r="AW3" s="14"/>
+      <c r="AX3" s="14"/>
     </row>
     <row r="4" spans="1:50" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="14"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1657,358 +1672,384 @@
       </c>
     </row>
     <row r="10" spans="1:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="22"/>
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="20"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="25"/>
     </row>
     <row r="12" spans="1:50" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="21"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="23"/>
-    </row>
-    <row r="14" spans="1:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="29" t="s">
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
+    </row>
+    <row r="13" spans="1:50" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+    </row>
+    <row r="15" spans="1:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C15" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="26"/>
-    </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="B15" s="29"/>
-      <c r="C15" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="27" t="s">
-        <v>22</v>
-      </c>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
       <c r="G15" s="30"/>
       <c r="H15" s="30"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
+      <c r="I15" s="11"/>
     </row>
     <row r="16" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="29"/>
+      <c r="C16" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B17" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D17" s="2">
         <v>3758</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F17" s="2">
         <v>3784</v>
       </c>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B17" s="24" t="s">
+      <c r="G17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="2">
+        <v>3816</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B18" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D18" s="2">
         <v>4440</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F18" s="2">
         <v>4481</v>
       </c>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B18" s="24" t="s">
+      <c r="G18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" s="2">
+        <v>4351</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B19" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="25">
+      <c r="C19" s="10">
         <v>2395</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D19" s="2">
         <v>2009</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F19" s="2">
         <v>2008</v>
       </c>
-      <c r="G18" s="34"/>
-      <c r="H18" s="33"/>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B19" s="24" t="s">
+      <c r="G19" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" s="10">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B20" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D20" s="2">
         <v>2316</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F20" s="2">
         <v>2299</v>
       </c>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="C21" s="1"/>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="F23" s="35"/>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B25" s="11" t="s">
+      <c r="G20" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" s="2">
+        <v>2339</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="C22" s="1"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="F24" s="13"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B26" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B26" s="8" t="s">
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B27" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C27" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9" t="s">
+      <c r="D27" s="19"/>
+      <c r="E27" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9" t="s">
+      <c r="F27" s="19"/>
+      <c r="G27" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9" t="s">
+      <c r="H27" s="19"/>
+      <c r="I27" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9" t="s">
+      <c r="J27" s="19"/>
+      <c r="K27" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9" t="s">
+      <c r="L27" s="19"/>
+      <c r="M27" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="N26" s="9"/>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B27" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="2">
-        <v>88</v>
-      </c>
-      <c r="D27" s="2">
-        <v>1.0056495666503911E-3</v>
-      </c>
-      <c r="E27" s="2">
-        <v>92</v>
-      </c>
-      <c r="F27" s="2">
-        <v>0</v>
-      </c>
-      <c r="G27" s="2">
-        <v>96</v>
-      </c>
-      <c r="H27" s="2">
-        <v>1.008272171020508E-3</v>
-      </c>
-      <c r="I27" s="2">
-        <v>610</v>
-      </c>
-      <c r="J27" s="2">
-        <v>7.9991817474365234E-3</v>
-      </c>
-      <c r="K27" s="2">
-        <v>710</v>
-      </c>
-      <c r="L27" s="2">
-        <v>2.16069221496582E-2</v>
-      </c>
-      <c r="M27" s="2">
-        <v>804</v>
-      </c>
-      <c r="N27" s="2">
-        <v>2.9676437377929691E-2</v>
-      </c>
+      <c r="N27" s="19"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B28" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28" s="2">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D28" s="2">
-        <v>1.2010812759399411E-2</v>
+        <v>1.0056495666503911E-3</v>
       </c>
       <c r="E28" s="2">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F28" s="2">
-        <v>1.099371910095215E-2</v>
+        <v>0</v>
       </c>
       <c r="G28" s="2">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="H28" s="2">
-        <v>8.0296993255615234E-3</v>
+        <v>1.008272171020508E-3</v>
       </c>
       <c r="I28" s="2">
-        <v>733</v>
+        <v>610</v>
       </c>
       <c r="J28" s="2">
-        <v>4.5169553756713867</v>
+        <v>7.9991817474365234E-3</v>
       </c>
       <c r="K28" s="2">
-        <v>817</v>
+        <v>710</v>
       </c>
       <c r="L28" s="2">
-        <v>4.6302993297576904</v>
+        <v>2.16069221496582E-2</v>
       </c>
       <c r="M28" s="2">
-        <v>872</v>
+        <v>804</v>
       </c>
       <c r="N28" s="2">
-        <v>4.7317337989807129</v>
+        <v>2.9676437377929691E-2</v>
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B29" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C29" s="2">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="D29" s="2">
-        <v>1.505851745605469E-3</v>
+        <v>1.2010812759399411E-2</v>
       </c>
       <c r="E29" s="2">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="F29" s="2">
-        <v>1.9998550415039058E-3</v>
+        <v>1.099371910095215E-2</v>
       </c>
       <c r="G29" s="2">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="H29" s="2">
-        <v>1.0011196136474609E-3</v>
+        <v>8.0296993255615234E-3</v>
       </c>
       <c r="I29" s="2">
-        <v>383</v>
+        <v>733</v>
       </c>
       <c r="J29" s="2">
-        <v>1.7922878265380859E-2</v>
+        <v>4.5169553756713867</v>
       </c>
       <c r="K29" s="2">
-        <v>468</v>
+        <v>817</v>
       </c>
       <c r="L29" s="2">
-        <v>3.0069828033447269E-2</v>
+        <v>4.6302993297576904</v>
       </c>
       <c r="M29" s="2">
-        <v>590</v>
+        <v>872</v>
       </c>
       <c r="N29" s="2">
-        <v>4.0013790130615227E-2</v>
+        <v>4.7317337989807129</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B30" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="2">
+        <v>66</v>
+      </c>
+      <c r="D30" s="2">
+        <v>1.505851745605469E-3</v>
+      </c>
+      <c r="E30" s="2">
+        <v>76</v>
+      </c>
+      <c r="F30" s="2">
+        <v>1.9998550415039058E-3</v>
+      </c>
+      <c r="G30" s="2">
+        <v>85</v>
+      </c>
+      <c r="H30" s="2">
+        <v>1.0011196136474609E-3</v>
+      </c>
+      <c r="I30" s="2">
+        <v>383</v>
+      </c>
+      <c r="J30" s="2">
+        <v>1.7922878265380859E-2</v>
+      </c>
+      <c r="K30" s="2">
+        <v>468</v>
+      </c>
+      <c r="L30" s="2">
+        <v>3.0069828033447269E-2</v>
+      </c>
+      <c r="M30" s="2">
+        <v>590</v>
+      </c>
+      <c r="N30" s="2">
+        <v>4.0013790130615227E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B31" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C31" s="2">
         <v>97</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D31" s="2">
         <v>1.0890960693359379E-3</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E31" s="2">
         <v>100</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F31" s="2">
         <v>2.0389556884765621E-3</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G31" s="2">
         <v>100</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H31" s="2">
         <v>5.0292015075683594E-3</v>
       </c>
-      <c r="I30" s="2">
+      <c r="I31" s="2">
         <v>562</v>
       </c>
-      <c r="J30" s="2">
+      <c r="J31" s="2">
         <v>5.0001144409179688E-3</v>
       </c>
-      <c r="K30" s="2">
+      <c r="K31" s="2">
         <v>702</v>
       </c>
-      <c r="L30" s="2">
+      <c r="L31" s="2">
         <v>1.8926858901977539E-2</v>
       </c>
-      <c r="M30" s="2">
+      <c r="M31" s="2">
         <v>871</v>
       </c>
-      <c r="N30" s="2">
+      <c r="N31" s="2">
         <v>3.3178329467773438E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="AQ2:AX2"/>
-    <mergeCell ref="AQ3:AT3"/>
-    <mergeCell ref="AU3:AX3"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="O3:R3"/>
-    <mergeCell ref="S3:V3"/>
-    <mergeCell ref="W3:Z3"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="B26:N26"/>
+    <mergeCell ref="B10:D12"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="K27:L27"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="AA3:AD3"/>
     <mergeCell ref="AE3:AH3"/>
@@ -2019,16 +2060,15 @@
     <mergeCell ref="S2:Z2"/>
     <mergeCell ref="AA2:AH2"/>
     <mergeCell ref="AI2:AP2"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="B25:N25"/>
-    <mergeCell ref="B10:D12"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="AQ2:AX2"/>
+    <mergeCell ref="AQ3:AT3"/>
+    <mergeCell ref="AU3:AX3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="O3:R3"/>
+    <mergeCell ref="S3:V3"/>
+    <mergeCell ref="W3:Z3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>